<commit_message>
gilbert ajout fichier wrover-cam
</commit_message>
<xml_diff>
--- a/Tableau_correspondance_pinsV2.xlsx
+++ b/Tableau_correspondance_pinsV2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sesa466660\Documents\Projet_frelons\Projet-frelons\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SESA638945\Documents\Projet_Frelon\Projet-frelons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378D1A16-E29A-42C1-A8C7-31265D24A3C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547279F5-E30D-4A8D-B54F-886431F0AD21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="153">
   <si>
     <t>ESP32 WROVER</t>
   </si>
@@ -412,6 +412,78 @@
   </si>
   <si>
     <t>TX televersement</t>
+  </si>
+  <si>
+    <t>SD_CLK</t>
+  </si>
+  <si>
+    <t>SD_D2</t>
+  </si>
+  <si>
+    <t>SD_D3</t>
+  </si>
+  <si>
+    <t>SD_D0</t>
+  </si>
+  <si>
+    <t>SD_D1</t>
+  </si>
+  <si>
+    <t>CA_D0</t>
+  </si>
+  <si>
+    <t>CA_D1</t>
+  </si>
+  <si>
+    <t>CA_D2</t>
+  </si>
+  <si>
+    <t>CA_D3</t>
+  </si>
+  <si>
+    <t>Nom pin schéma</t>
+  </si>
+  <si>
+    <t>CA_D4</t>
+  </si>
+  <si>
+    <t>CA_D5</t>
+  </si>
+  <si>
+    <t>CA_D6</t>
+  </si>
+  <si>
+    <t>CA_D7</t>
+  </si>
+  <si>
+    <t>CA_VSYNC</t>
+  </si>
+  <si>
+    <t>CA_SIO_D</t>
+  </si>
+  <si>
+    <t>CA_SIO_C</t>
+  </si>
+  <si>
+    <t>SD_CMD</t>
+  </si>
+  <si>
+    <t>CA_D0_SD_D1</t>
+  </si>
+  <si>
+    <t>CA_XCLK_SD_DET</t>
+  </si>
+  <si>
+    <t>CA_HREF</t>
+  </si>
+  <si>
+    <t>CA_PCLK</t>
+  </si>
+  <si>
+    <t>CA_RESET</t>
+  </si>
+  <si>
+    <t>CA_RST_SD_CMD</t>
   </si>
 </sst>
 </file>
@@ -427,7 +499,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -512,6 +584,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -562,7 +640,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -667,6 +745,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1058,31 +1139,32 @@
   <dimension ref="A1:AMH46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="1"/>
-    <col min="3" max="3" width="6.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" style="1"/>
+    <col min="3" max="3" width="6.5546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="33" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="5.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="5.44140625" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" style="1" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="8" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="22.85546875" style="1" customWidth="1"/>
-    <col min="13" max="14" width="11.42578125" style="1"/>
+    <col min="11" max="11" width="10.5546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="22.88671875" style="1" customWidth="1"/>
+    <col min="13" max="14" width="11.44140625" style="1"/>
     <col min="15" max="15" width="20" style="1" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" style="1" customWidth="1"/>
-    <col min="17" max="1022" width="11.42578125" style="1"/>
-    <col min="1023" max="1024" width="11.42578125"/>
+    <col min="16" max="16" width="18.6640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="20.21875" style="1" customWidth="1"/>
+    <col min="18" max="1022" width="11.44140625" style="1"/>
+    <col min="1023" max="1024" width="11.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
@@ -1105,8 +1187,9 @@
       <c r="N1" s="35"/>
       <c r="O1" s="35"/>
       <c r="P1" s="35"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" s="35"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1155,8 +1238,11 @@
       <c r="P2" s="32" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" s="36" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1183,8 +1269,9 @@
       <c r="N3" s="2"/>
       <c r="O3" s="29"/>
       <c r="P3" s="8"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" s="8"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -1211,8 +1298,9 @@
       <c r="N4" s="2"/>
       <c r="O4" s="29"/>
       <c r="P4" s="8"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4" s="8"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -1239,8 +1327,9 @@
       <c r="N5" s="2"/>
       <c r="O5" s="29"/>
       <c r="P5" s="8"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q5" s="8"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -1269,8 +1358,11 @@
       <c r="N6" s="2"/>
       <c r="O6" s="29"/>
       <c r="P6" s="8"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q6" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1299,8 +1391,11 @@
       <c r="N7" s="2"/>
       <c r="O7" s="29"/>
       <c r="P7" s="8"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q7" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -1329,8 +1424,11 @@
       <c r="N8" s="2"/>
       <c r="O8" s="29"/>
       <c r="P8" s="8"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q8" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
@@ -1359,8 +1457,11 @@
       <c r="N9" s="2"/>
       <c r="O9" s="29"/>
       <c r="P9" s="8"/>
-    </row>
-    <row r="10" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="Q9" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
@@ -1391,8 +1492,11 @@
         <v>122</v>
       </c>
       <c r="P10" s="8"/>
-    </row>
-    <row r="11" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="Q10" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>34</v>
       </c>
@@ -1423,8 +1527,11 @@
         <v>121</v>
       </c>
       <c r="P11" s="8"/>
-    </row>
-    <row r="12" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q11" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
@@ -1453,8 +1560,11 @@
       <c r="N12" s="2"/>
       <c r="O12" s="29"/>
       <c r="P12" s="8"/>
-    </row>
-    <row r="13" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q12" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>37</v>
       </c>
@@ -1483,8 +1593,11 @@
       <c r="N13" s="2"/>
       <c r="O13" s="29"/>
       <c r="P13" s="8"/>
-    </row>
-    <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q13" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>39</v>
       </c>
@@ -1513,8 +1626,11 @@
       <c r="N14" s="2"/>
       <c r="O14" s="29"/>
       <c r="P14" s="8"/>
-    </row>
-    <row r="15" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="Q14" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
@@ -1541,14 +1657,17 @@
       </c>
       <c r="K15" s="8"/>
       <c r="L15" s="23" t="s">
-        <v>42</v>
+        <v>129</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="29"/>
       <c r="P15" s="8"/>
-    </row>
-    <row r="16" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="Q15" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>44</v>
       </c>
@@ -1575,14 +1694,17 @@
       </c>
       <c r="K16" s="8"/>
       <c r="L16" s="23" t="s">
-        <v>45</v>
+        <v>130</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="29"/>
       <c r="P16" s="8"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q16" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -1609,8 +1731,9 @@
       <c r="N17" s="2"/>
       <c r="O17" s="29"/>
       <c r="P17" s="8"/>
-    </row>
-    <row r="18" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="Q17" s="8"/>
+    </row>
+    <row r="18" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>47</v>
       </c>
@@ -1637,14 +1760,17 @@
       </c>
       <c r="K18" s="8"/>
       <c r="L18" s="23" t="s">
-        <v>48</v>
+        <v>131</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="29"/>
       <c r="P18" s="8"/>
-    </row>
-    <row r="19" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q18" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>50</v>
       </c>
@@ -1673,8 +1799,9 @@
       <c r="N19" s="11"/>
       <c r="O19" s="30"/>
       <c r="P19" s="8"/>
-    </row>
-    <row r="20" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q19" s="8"/>
+    </row>
+    <row r="20" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>53</v>
       </c>
@@ -1703,8 +1830,9 @@
       <c r="N20" s="11"/>
       <c r="O20" s="30"/>
       <c r="P20" s="8"/>
-    </row>
-    <row r="21" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q20" s="8"/>
+    </row>
+    <row r="21" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>54</v>
       </c>
@@ -1733,8 +1861,9 @@
       <c r="N21" s="11"/>
       <c r="O21" s="30"/>
       <c r="P21" s="8"/>
-    </row>
-    <row r="22" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q21" s="8"/>
+    </row>
+    <row r="22" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>55</v>
       </c>
@@ -1763,8 +1892,9 @@
       <c r="N22" s="11"/>
       <c r="O22" s="30"/>
       <c r="P22" s="8"/>
-    </row>
-    <row r="23" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q22" s="8"/>
+    </row>
+    <row r="23" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>56</v>
       </c>
@@ -1793,8 +1923,9 @@
       <c r="N23" s="11"/>
       <c r="O23" s="30"/>
       <c r="P23" s="8"/>
-    </row>
-    <row r="24" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q23" s="8"/>
+    </row>
+    <row r="24" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>57</v>
       </c>
@@ -1823,8 +1954,9 @@
       <c r="N24" s="11"/>
       <c r="O24" s="30"/>
       <c r="P24" s="8"/>
-    </row>
-    <row r="25" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="Q24" s="8"/>
+    </row>
+    <row r="25" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>58</v>
       </c>
@@ -1849,16 +1981,21 @@
       <c r="J25" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="K25" s="20"/>
+      <c r="K25" s="22" t="s">
+        <v>65</v>
+      </c>
       <c r="L25" s="9" t="s">
-        <v>59</v>
+        <v>146</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="29"/>
       <c r="P25" s="8"/>
-    </row>
-    <row r="26" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="Q25" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>61</v>
       </c>
@@ -1885,14 +2022,17 @@
       </c>
       <c r="K26" s="20"/>
       <c r="L26" s="9" t="s">
-        <v>62</v>
+        <v>132</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="29"/>
       <c r="P26" s="8"/>
-    </row>
-    <row r="27" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="Q26" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>64</v>
       </c>
@@ -1915,16 +2055,16 @@
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
-      <c r="K27" s="22" t="s">
-        <v>65</v>
-      </c>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="29"/>
       <c r="P27" s="8"/>
-    </row>
-    <row r="28" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="Q27" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>67</v>
       </c>
@@ -1950,17 +2090,20 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="22" t="s">
-        <v>68</v>
+        <v>134</v>
       </c>
       <c r="L28" s="9" t="s">
-        <v>69</v>
+        <v>133</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" s="29"/>
       <c r="P28" s="8"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q28" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>71</v>
       </c>
@@ -1987,8 +2130,9 @@
       <c r="N29" s="2"/>
       <c r="O29" s="29"/>
       <c r="P29" s="8"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q29" s="8"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>73</v>
       </c>
@@ -2015,8 +2159,9 @@
       <c r="N30" s="2"/>
       <c r="O30" s="29"/>
       <c r="P30" s="8"/>
-    </row>
-    <row r="31" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q30" s="8"/>
+    </row>
+    <row r="31" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>74</v>
       </c>
@@ -2045,8 +2190,11 @@
       <c r="N31" s="2"/>
       <c r="O31" s="29"/>
       <c r="P31" s="8"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q31" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>76</v>
       </c>
@@ -2075,8 +2223,11 @@
       <c r="N32" s="2"/>
       <c r="O32" s="29"/>
       <c r="P32" s="8"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q32" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>78</v>
       </c>
@@ -2105,8 +2256,11 @@
       <c r="N33" s="2"/>
       <c r="O33" s="29"/>
       <c r="P33" s="8"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q33" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>80</v>
       </c>
@@ -2133,8 +2287,9 @@
       <c r="N34" s="26"/>
       <c r="O34" s="31"/>
       <c r="P34" s="8"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q34" s="8"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="14" t="s">
         <v>81</v>
       </c>
@@ -2167,8 +2322,11 @@
       <c r="N35" s="2"/>
       <c r="O35" s="29"/>
       <c r="P35" s="8"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q35" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>84</v>
       </c>
@@ -2195,8 +2353,9 @@
       <c r="P36" s="32" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q36" s="8"/>
+    </row>
+    <row r="37" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>85</v>
       </c>
@@ -2223,8 +2382,9 @@
       <c r="P37" s="32" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q37" s="8"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="14" t="s">
         <v>86</v>
       </c>
@@ -2253,8 +2413,11 @@
       <c r="N38" s="2"/>
       <c r="O38" s="29"/>
       <c r="P38" s="8"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q38" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>88</v>
       </c>
@@ -2283,8 +2446,11 @@
       <c r="N39" s="2"/>
       <c r="O39" s="29"/>
       <c r="P39" s="8"/>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q39" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>13</v>
       </c>
@@ -2309,8 +2475,11 @@
       <c r="N40" s="2"/>
       <c r="O40" s="29"/>
       <c r="P40" s="8"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q40" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2329,8 +2498,9 @@
       <c r="N41" s="2"/>
       <c r="O41" s="29"/>
       <c r="P41" s="8"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q41" s="8"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -2351,8 +2521,9 @@
       <c r="N42" s="2"/>
       <c r="O42" s="29"/>
       <c r="P42" s="8"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q42" s="8"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>7</v>
       </c>
@@ -2371,7 +2542,7 @@
       <c r="N44" s="16"/>
       <c r="O44" s="16"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>10</v>
       </c>
@@ -2390,7 +2561,7 @@
       <c r="N45" s="18"/>
       <c r="O45" s="18"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>9</v>
       </c>
@@ -2402,7 +2573,7 @@
   <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:I1"/>
-    <mergeCell ref="J1:P1"/>
+    <mergeCell ref="J1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Mis a jour fait par Gilbert Kagbadouno
</commit_message>
<xml_diff>
--- a/Tableau_correspondance_pinsV2.xlsx
+++ b/Tableau_correspondance_pinsV2.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sesa466660\Documents\Projet_frelons\Projet-frelons\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SESA638945\Documents\Projet_Frelon\Projet-frelons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74442B47-3CB1-4016-9134-8BB661FDFEA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC955F9-A049-4E04-AA89-88ED2FD8ECD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="154">
   <si>
     <t>ESP32 WROVER</t>
   </si>
@@ -1141,33 +1141,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMH46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="1"/>
-    <col min="3" max="3" width="6.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" style="1"/>
+    <col min="3" max="3" width="6.5546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="33" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="1" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="5.42578125" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="5.44140625" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" style="1" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="8" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="22.85546875" style="1" customWidth="1"/>
-    <col min="13" max="14" width="11.42578125" style="1"/>
+    <col min="11" max="11" width="10.5546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="22.88671875" style="1" customWidth="1"/>
+    <col min="13" max="14" width="11.44140625" style="1"/>
     <col min="15" max="15" width="20" style="1" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="20.28515625" style="1" customWidth="1"/>
-    <col min="18" max="1022" width="11.42578125" style="1"/>
-    <col min="1023" max="1024" width="11.42578125"/>
+    <col min="16" max="16" width="18.6640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="20.33203125" style="1" customWidth="1"/>
+    <col min="18" max="1022" width="11.44140625" style="1"/>
+    <col min="1023" max="1024" width="11.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
@@ -1192,7 +1192,7 @@
       <c r="P1" s="36"/>
       <c r="Q1" s="36"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1274,7 +1274,7 @@
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -1303,7 +1303,7 @@
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -1332,7 +1332,7 @@
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>34</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>37</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>39</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
@@ -1658,7 +1658,9 @@
       <c r="J15" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="K15" s="8"/>
+      <c r="K15" s="22" t="s">
+        <v>153</v>
+      </c>
       <c r="L15" s="23" t="s">
         <v>129</v>
       </c>
@@ -1670,7 +1672,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>44</v>
       </c>
@@ -1707,7 +1709,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -1736,7 +1738,7 @@
       <c r="P17" s="8"/>
       <c r="Q17" s="8"/>
     </row>
-    <row r="18" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>47</v>
       </c>
@@ -1773,7 +1775,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>50</v>
       </c>
@@ -1804,7 +1806,7 @@
       <c r="P19" s="8"/>
       <c r="Q19" s="8"/>
     </row>
-    <row r="20" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>53</v>
       </c>
@@ -1835,7 +1837,7 @@
       <c r="P20" s="8"/>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>54</v>
       </c>
@@ -1866,7 +1868,7 @@
       <c r="P21" s="8"/>
       <c r="Q21" s="8"/>
     </row>
-    <row r="22" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>55</v>
       </c>
@@ -1897,7 +1899,7 @@
       <c r="P22" s="8"/>
       <c r="Q22" s="8"/>
     </row>
-    <row r="23" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>56</v>
       </c>
@@ -1928,7 +1930,7 @@
       <c r="P23" s="8"/>
       <c r="Q23" s="8"/>
     </row>
-    <row r="24" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>57</v>
       </c>
@@ -1959,7 +1961,7 @@
       <c r="P24" s="8"/>
       <c r="Q24" s="8"/>
     </row>
-    <row r="25" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>58</v>
       </c>
@@ -1998,7 +2000,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>61</v>
       </c>
@@ -2035,7 +2037,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>64</v>
       </c>
@@ -2067,7 +2069,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>67</v>
       </c>
@@ -2106,7 +2108,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>71</v>
       </c>
@@ -2135,7 +2137,7 @@
       <c r="P29" s="8"/>
       <c r="Q29" s="8"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>73</v>
       </c>
@@ -2164,7 +2166,7 @@
       <c r="P30" s="8"/>
       <c r="Q30" s="8"/>
     </row>
-    <row r="31" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>74</v>
       </c>
@@ -2197,7 +2199,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>76</v>
       </c>
@@ -2230,7 +2232,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>78</v>
       </c>
@@ -2263,7 +2265,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>80</v>
       </c>
@@ -2292,7 +2294,7 @@
       <c r="P34" s="8"/>
       <c r="Q34" s="8"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="14" t="s">
         <v>81</v>
       </c>
@@ -2329,7 +2331,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>84</v>
       </c>
@@ -2358,7 +2360,7 @@
       </c>
       <c r="Q36" s="8"/>
     </row>
-    <row r="37" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>85</v>
       </c>
@@ -2387,7 +2389,7 @@
       </c>
       <c r="Q37" s="8"/>
     </row>
-    <row r="38" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="14" t="s">
         <v>86</v>
       </c>
@@ -2420,7 +2422,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>88</v>
       </c>
@@ -2453,7 +2455,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>13</v>
       </c>
@@ -2482,7 +2484,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2503,7 +2505,7 @@
       <c r="P41" s="8"/>
       <c r="Q41" s="8"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -2528,7 +2530,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>7</v>
       </c>
@@ -2547,7 +2549,7 @@
       <c r="N44" s="16"/>
       <c r="O44" s="16"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>10</v>
       </c>
@@ -2566,7 +2568,7 @@
       <c r="N45" s="18"/>
       <c r="O45" s="18"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>9</v>
       </c>

</xml_diff>